<commit_message>
feat: add upload csv supply service
</commit_message>
<xml_diff>
--- a/api/utils/templates/xlsx/baseSupplyUploadResponse.xlsx
+++ b/api/utils/templates/xlsx/baseSupplyUploadResponse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugod\Desktop\proyectos\maximport\sources\max-import-backend\api\utils\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EF3885-4167-4C67-A162-ABFA24E698A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CB5150-6473-4725-8257-C1FD5E684B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F90E08B-5E6B-4E95-9F51-698F115049C6}"/>
   </bookViews>
@@ -34,36 +34,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">CODIGO </t>
   </si>
   <si>
-    <t>FAMILIA</t>
-  </si>
-  <si>
-    <t>SUBFAMILIA</t>
-  </si>
-  <si>
-    <t>ELEMENTO</t>
-  </si>
-  <si>
-    <t>MODELO</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>UPLOAD</t>
-  </si>
-  <si>
-    <t>MOTIVO</t>
-  </si>
-  <si>
-    <t>PROVEEDOR</t>
-  </si>
-  <si>
     <t>CARGA MASIVA DE ABASTECIMIENTO</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>Almacen</t>
+  </si>
+  <si>
+    <t>Código de Carga</t>
+  </si>
+  <si>
+    <t>Fecha de llegada</t>
+  </si>
+  <si>
+    <t>PRODUCTOS</t>
+  </si>
+  <si>
+    <t>CANTIDAD CAJAS</t>
+  </si>
+  <si>
+    <t>UNIDADES POR CAJA</t>
   </si>
 </sst>
 </file>
@@ -113,9 +110,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -435,17 +439,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF94AF20-A2FF-4736-94BE-B00DDB288A13}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
@@ -455,45 +459,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>